<commit_message>
add inputs (example), pathdinfer and demand notebook
</commit_message>
<xml_diff>
--- a/inputs/parameters.xlsx
+++ b/inputs/parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t xml:space="preserve">Fichier de paramètre du modèle Quetzal Montréal</t>
   </si>
@@ -274,7 +274,13 @@
     <t xml:space="preserve">base</t>
   </si>
   <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
     <t xml:space="preserve">am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pm</t>
   </si>
   <si>
     <t xml:space="preserve">general</t>
@@ -827,10 +833,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topRight" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="33.71"/>
@@ -867,6 +873,12 @@
       </c>
       <c r="H1" s="13" t="s">
         <v>29</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="ACE1" s="0"/>
       <c r="ACF1" s="0"/>
@@ -1137,14 +1149,14 @@
     </row>
     <row r="2" s="15" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1152,6 +1164,12 @@
         <v>28</v>
       </c>
       <c r="H2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="ACE2" s="0"/>
@@ -1423,19 +1441,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G3" s="12" t="n">
         <v>500</v>
@@ -1444,19 +1462,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="G4" s="12" t="n">
         <f aca="false">4/SQRT(2)</f>
@@ -1466,16 +1484,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G5" s="12" t="n">
         <v>4</v>
@@ -1484,16 +1502,16 @@
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G6" s="12" t="n">
         <f aca="false">4/SQRT(2)</f>
@@ -1503,16 +1521,16 @@
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7" s="12" t="n">
         <v>5000</v>
@@ -1521,16 +1539,16 @@
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G8" s="12" t="n">
         <f aca="false">30</f>

</xml_diff>

<commit_message>
change for immense inputs
</commit_message>
<xml_diff>
--- a/inputs/parameters.xlsx
+++ b/inputs/parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t xml:space="preserve">Fichier de paramètre du modèle Quetzal Montréal</t>
   </si>
@@ -281,6 +281,12 @@
   </si>
   <si>
     <t xml:space="preserve">pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">op</t>
   </si>
   <si>
     <t xml:space="preserve">general</t>
@@ -831,12 +837,12 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="33.71"/>
@@ -879,6 +885,12 @@
       </c>
       <c r="J1" s="15" t="s">
         <v>31</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="ACE1" s="0"/>
       <c r="ACF1" s="0"/>
@@ -1149,14 +1161,14 @@
     </row>
     <row r="2" s="15" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -1170,6 +1182,12 @@
         <v>28</v>
       </c>
       <c r="J2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>28</v>
       </c>
       <c r="ACE2" s="0"/>
@@ -1441,19 +1459,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G3" s="12" t="n">
         <v>500</v>
@@ -1462,19 +1480,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="G4" s="12" t="n">
         <f aca="false">4/SQRT(2)</f>
@@ -1484,16 +1502,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G5" s="12" t="n">
         <v>4</v>
@@ -1502,16 +1520,16 @@
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" s="12" t="n">
         <f aca="false">4/SQRT(2)</f>
@@ -1521,34 +1539,34 @@
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7" s="12" t="n">
-        <v>5000</v>
+        <v>10000000000</v>
       </c>
       <c r="H7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G8" s="12" t="n">
         <f aca="false">30</f>

</xml_diff>